<commit_message>
Primera verificacion hasta el punto 10
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Escenario</t>
   </si>
@@ -74,6 +74,39 @@
   </si>
   <si>
     <t>RESOPT[%]</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98011 SGDEHI0713.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98012 SGDEHI0813.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98013 SGDEHI0913.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98014 SGDEHI1013.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98015 SGDEHI1113.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98016 SGDEHI1213.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98017  SGDEHI1413.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 99 U.T.E NO POSEE SYSTEMA</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 18 A.N.D.E. NO POSEE SYSTEMA</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 20 BRASIL NO POSEE SYSTEMA</t>
   </si>
 </sst>
 </file>
@@ -606,7 +639,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -703,59 +736,30 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="n">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>899.9999761581421</v>
+        <v>800.4000333607197</v>
       </c>
       <c r="E4" t="n">
-        <v>799.9994506835938</v>
+        <v>579.9990844726562</v>
       </c>
       <c r="F4" t="n">
-        <v>100.0005254745483</v>
+        <v>220.4009488880635</v>
       </c>
       <c r="G4" t="n">
-        <v>12.50007426743839</v>
+        <v>38.00022358456915</v>
       </c>
       <c r="H4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="n">
-        <v>211</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>800.4000333607197</v>
-      </c>
-      <c r="E5" t="n">
-        <v>579.9990844726562</v>
-      </c>
-      <c r="F5" t="n">
-        <v>220.4009488880635</v>
-      </c>
-      <c r="G5" t="n">
-        <v>38.00022358456915</v>
-      </c>
-      <c r="H5" t="n">
-        <v>10</v>
-      </c>
-      <c r="I5" t="n">
         <v>15</v>
       </c>
     </row>
@@ -880,7 +884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -888,18 +892,94 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada la descripcion de los informes
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -532,7 +532,7 @@
         <v>195.000994682312</v>
       </c>
       <c r="G2" t="n">
-        <v>26.0001685945936</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>
@@ -561,7 +561,7 @@
         <v>195.000994682312</v>
       </c>
       <c r="G3" t="n">
-        <v>26.0001685945936</v>
+        <v>26</v>
       </c>
       <c r="H3" t="n">
         <v>5</v>
@@ -590,7 +590,7 @@
         <v>100.0005254745483</v>
       </c>
       <c r="G4" t="n">
-        <v>12.50007426743839</v>
+        <v>12.5</v>
       </c>
       <c r="H4" t="n">
         <v>5</v>
@@ -619,7 +619,7 @@
         <v>220.4009488880635</v>
       </c>
       <c r="G5" t="n">
-        <v>38.00022358456915</v>
+        <v>38</v>
       </c>
       <c r="H5" t="n">
         <v>10</v>
@@ -696,7 +696,7 @@
         <v>195.000994682312</v>
       </c>
       <c r="G2" t="n">
-        <v>26.0001685945936</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>
@@ -725,7 +725,7 @@
         <v>195.000994682312</v>
       </c>
       <c r="G3" t="n">
-        <v>26.0001685945936</v>
+        <v>26</v>
       </c>
       <c r="H3" t="n">
         <v>5</v>
@@ -754,7 +754,7 @@
         <v>220.4009488880635</v>
       </c>
       <c r="G4" t="n">
-        <v>38.00022358456915</v>
+        <v>38</v>
       </c>
       <c r="H4" t="n">
         <v>10</v>
@@ -831,7 +831,7 @@
         <v>100.0005254745483</v>
       </c>
       <c r="G2" t="n">
-        <v>12.50007426743839</v>
+        <v>12.5</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
modificacion del informe reserva_total
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,7 +20,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+  <si>
+    <t>Análisis de la Reserva Total</t>
+  </si>
+  <si>
+    <t>RESERVA ROTANTE EN MAQUINAS QUE REGULAN</t>
+  </si>
+  <si>
+    <t>RESERVA HIDRO [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA TERMICA [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA TOTAL [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA ROTANTE DEL PARQUE REGULANTE</t>
+  </si>
+  <si>
+    <t>RESERVA HIDRO</t>
+  </si>
+  <si>
+    <t>RESERVA PROGRAMADA A 50Hz PARA RPF</t>
+  </si>
+  <si>
+    <t>RESERVA TÉRMICA</t>
+  </si>
+  <si>
+    <t>TOTAL SISTEMA</t>
+  </si>
+  <si>
+    <t>RESERVA PARA RPF</t>
+  </si>
+  <si>
+    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [MW]</t>
+  </si>
+  <si>
+    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [%]</t>
+  </si>
+  <si>
+    <t>POTENCIA OPERABLE EN EL PARQUE REGULANTE</t>
+  </si>
+  <si>
+    <t>HIDRO</t>
+  </si>
+  <si>
+    <t>TÉRMICA TG-CC</t>
+  </si>
+  <si>
+    <t>TÉRMICA TV</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>RESERVA PROGRAMADA EN EL PARQUE REGULANTE</t>
+  </si>
+  <si>
+    <t>RESERVA NUEVA</t>
+  </si>
+  <si>
+    <t>RESERVA TOTAL 2</t>
+  </si>
+  <si>
+    <t>IBUS</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>POT_MAX[MW]</t>
+  </si>
+  <si>
+    <t>POT_GEN[MW]</t>
+  </si>
+  <si>
+    <t>MAX_GEN[MW]</t>
+  </si>
+  <si>
+    <t>RESERVA_DATO[%]</t>
+  </si>
+  <si>
+    <t>PORCENTAJE[%]</t>
+  </si>
+  <si>
+    <t>RES_OPT[%]</t>
+  </si>
+  <si>
+    <t>NUC-A       21.600</t>
+  </si>
+  <si>
+    <t>NUC-B       21.600</t>
+  </si>
+  <si>
+    <t>URBGEN      18.000</t>
+  </si>
+  <si>
+    <t>HYDRO_G     20.000</t>
+  </si>
+  <si>
+    <t>RESOPT[%]</t>
+  </si>
   <si>
     <t>Escenario</t>
   </si>
@@ -34,49 +139,37 @@
     <t>Reserva Total</t>
   </si>
   <si>
-    <t>IBUS</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>POT_MAX[MW]</t>
-  </si>
-  <si>
-    <t>POT_GEN[MW]</t>
-  </si>
-  <si>
-    <t>MAX_GEN[MW]</t>
-  </si>
-  <si>
-    <t>RESERVA_DATO[%]</t>
-  </si>
-  <si>
-    <t>PORCENTAJE[%]</t>
-  </si>
-  <si>
-    <t>RES_OPT[%]</t>
-  </si>
-  <si>
-    <t>NUC-A       21.600</t>
-  </si>
-  <si>
-    <t>NUC-B       21.600</t>
-  </si>
-  <si>
-    <t>URBGEN      18.000</t>
-  </si>
-  <si>
-    <t>HYDRO_G     20.000</t>
-  </si>
-  <si>
-    <t>RESOPT[%]</t>
-  </si>
-  <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98011 SGDEHI0713.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98012 SGDEHI0813.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98013 SGDEHI0913.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98014 SGDEHI1013.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98015 SGDEHI1113.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98016 SGDEHI1213.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE GENSALE.PRN ***** NO SE ENCUENTRA LA BARRA 98017  SGDEHI1413.8</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 99 U.T.E NO POSEE SYSTEMA</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 18 A.N.D.E. NO POSEE SYSTEMA</t>
+  </si>
+  <si>
+    <t>***** ERROR EN LOS DATOS DE reserva_DEMANDAS ***** EL AREA INDICADA COMO 20 BRASIL NO POSEE SYSTEMA</t>
   </si>
 </sst>
 </file>
@@ -101,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,12 +202,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -412,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,21 +523,169 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="n"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A21:F21"/>
+  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -455,31 +706,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -487,7 +738,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -516,7 +767,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -545,7 +796,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -574,7 +825,7 @@
         <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -619,31 +870,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -651,7 +902,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -680,7 +931,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -709,7 +960,7 @@
         <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -754,31 +1005,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -786,7 +1037,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -831,16 +1082,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +1105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,7 +1115,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casi terminado informe total reserva
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -40,10 +40,10 @@
     <t>RESERVA ROTANTE DEL PARQUE REGULANTE</t>
   </si>
   <si>
+    <t>RESERVA PROGRAMADA A 50Hz PARA RPF</t>
+  </si>
+  <si>
     <t>RESERVA HIDRO</t>
-  </si>
-  <si>
-    <t>RESERVA PROGRAMADA A 50Hz PARA RPF</t>
   </si>
   <si>
     <t>RESERVA TÉRMICA</t>
@@ -213,9 +213,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,19 +557,19 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
-      <c r="E7" s="1" t="n"/>
-      <c r="F7" s="1" t="n"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -575,106 +578,96 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>12</v>
+      <c r="A15" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
-      <c r="D16" s="1" t="n"/>
-      <c r="E16" s="1" t="n"/>
-      <c r="F16" s="1" t="n"/>
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n"/>
-      <c r="E21" s="1" t="n"/>
-      <c r="F21" s="1" t="n"/>
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="36">
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:F4"/>
@@ -682,9 +675,35 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Verificada la potencia del sistema
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,70 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
-  <si>
-    <t>Análisis de la Reserva Total</t>
-  </si>
-  <si>
-    <t>RESERVA ROTANTE EN MAQUINAS QUE REGULAN</t>
-  </si>
-  <si>
-    <t>RESERVA HIDRO [MW]</t>
-  </si>
-  <si>
-    <t>RESERVA TERMICA [MW]</t>
-  </si>
-  <si>
-    <t>RESERVA TOTAL [MW]</t>
-  </si>
-  <si>
-    <t>RESERVA ROTANTE DEL PARQUE REGULANTE</t>
-  </si>
-  <si>
-    <t>RESERVA PROGRAMADA A 50Hz PARA RPF</t>
-  </si>
-  <si>
-    <t>RESERVA HIDRO</t>
-  </si>
-  <si>
-    <t>RESERVA TÉRMICA</t>
-  </si>
-  <si>
-    <t>TOTAL SISTEMA</t>
-  </si>
-  <si>
-    <t>RESERVA PARA RPF</t>
-  </si>
-  <si>
-    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [MW]</t>
-  </si>
-  <si>
-    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [%]</t>
-  </si>
-  <si>
-    <t>POTENCIA OPERABLE EN EL PARQUE REGULANTE</t>
-  </si>
-  <si>
-    <t>HIDRO</t>
-  </si>
-  <si>
-    <t>TÉRMICA TG-CC</t>
-  </si>
-  <si>
-    <t>TÉRMICA TV</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>RESERVA PROGRAMADA EN EL PARQUE REGULANTE</t>
-  </si>
-  <si>
-    <t>RESERVA NUEVA</t>
-  </si>
-  <si>
-    <t>RESERVA TOTAL 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>IBUS</t>
   </si>
@@ -194,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -202,25 +139,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -518,193 +442,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
-      <c r="E8" s="1" t="n"/>
-      <c r="F8" s="1" t="n"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="n"/>
-      <c r="F20" s="1" t="n"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -725,31 +470,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -757,7 +502,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -786,7 +531,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -815,7 +560,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -844,7 +589,7 @@
         <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -889,31 +634,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -921,7 +666,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -950,7 +695,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -979,7 +724,7 @@
         <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -1024,31 +769,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1056,7 +801,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -1101,16 +846,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1134,92 +879,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminado hasta el primer informe
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,7 +20,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+  <si>
+    <t>Análisis de la Reserva Total</t>
+  </si>
+  <si>
+    <t>RESERVA ROTANTE EN MAQUINAS QUE REGULAN</t>
+  </si>
+  <si>
+    <t>RESERVA HIDRO [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA TERMICA [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA TOTAL [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA ROTANTE DEL PARQUE REGULANTE [%]</t>
+  </si>
+  <si>
+    <t>RESERVA PROGRAMADA A 50Hz PARA RPF</t>
+  </si>
+  <si>
+    <t>RESERVA TÉRMICA [MW]</t>
+  </si>
+  <si>
+    <t>TOTAL SISTEMA [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA PARA RPF [%]</t>
+  </si>
+  <si>
+    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [MW]</t>
+  </si>
+  <si>
+    <t>COLABORACIÓN DEL PARQUE HIDRO EN RSF [%]</t>
+  </si>
+  <si>
+    <t>POTENCIA OPERABLE EN EL PARQUE REGULANTE</t>
+  </si>
+  <si>
+    <t>HIDRO [MW]</t>
+  </si>
+  <si>
+    <t>TÉRMICA TG-CC [MW]</t>
+  </si>
+  <si>
+    <t>TÉRMICA TV [MW]</t>
+  </si>
+  <si>
+    <t>TOTAL [MW]</t>
+  </si>
+  <si>
+    <t>RESERVA PROGRAMADA EN EL PARQUE REGULANTE</t>
+  </si>
+  <si>
+    <t>HIDRO</t>
+  </si>
+  <si>
+    <t>TÉRMICA TG-CC</t>
+  </si>
+  <si>
+    <t>TÉRMICA TV</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>RESERVA NUEVA</t>
+  </si>
+  <si>
+    <t>RESERVA TOTAL 2</t>
+  </si>
   <si>
     <t>IBUS</t>
   </si>
@@ -131,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,12 +211,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -442,14 +527,253 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>515.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>710.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>21.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="n">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="n">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1745.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3590.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="n">
+        <v>415.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="n">
+        <v>515.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="n">
+        <v>488.5525634765625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="n">
+        <v>610.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -470,31 +794,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -502,7 +826,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -531,7 +855,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -560,7 +884,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -589,7 +913,7 @@
         <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -634,31 +958,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -666,7 +990,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -695,7 +1019,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -724,7 +1048,7 @@
         <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -769,31 +1093,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -801,7 +1125,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -846,16 +1170,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -879,92 +1203,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solucionado el tema del recorte
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Análisis de la Reserva Total</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>RESERVA TOTAL 2 [MW]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUEGO DEL RECORTE DE PONTECIA MAXIMA EN LOS GENERADORES EN BASE A </t>
+  </si>
+  <si>
+    <t>RESERVA ROTANTE EN MÁQUINAS QUE REGULAN</t>
   </si>
   <si>
     <t>IBUS</t>
@@ -515,7 +521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,11 +538,6 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -574,11 +575,6 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
-      <c r="E8" s="1" t="n"/>
-      <c r="F8" s="1" t="n"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -629,7 +625,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -669,11 +665,6 @@
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="n"/>
-      <c r="F20" s="1" t="n"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
@@ -700,10 +691,10 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="1" t="n">
         <v>515.4</v>
       </c>
     </row>
@@ -711,10 +702,6 @@
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
-      <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n">
         <v>488.5525634765625</v>
       </c>
@@ -723,16 +710,229 @@
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="1" t="n"/>
-      <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n">
         <v>610.4</v>
       </c>
     </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>195.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="n">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="n"/>
+      <c r="C35" s="1" t="n"/>
+      <c r="D35" s="1" t="n"/>
+      <c r="E35" s="1" t="n"/>
+      <c r="F35" s="1" t="n"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="n">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="n">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="1" t="n"/>
+      <c r="E42" s="1" t="n"/>
+      <c r="F42" s="1" t="n"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="n">
+        <v>787.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1425.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="n"/>
+      <c r="D47" s="1" t="n"/>
+      <c r="E47" s="1" t="n"/>
+      <c r="F47" s="1" t="n"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="n">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="1" t="n"/>
+      <c r="C51" s="1" t="n"/>
+      <c r="D51" s="1" t="n">
+        <v>195.5</v>
+      </c>
+      <c r="E51" s="1" t="n"/>
+      <c r="F51" s="1" t="n"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="n"/>
+      <c r="D52" s="1" t="n"/>
+      <c r="E52" s="1" t="n"/>
+      <c r="F52" s="1" t="n">
+        <v>488.5525634765625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1" t="n"/>
+      <c r="C53" s="1" t="n"/>
+      <c r="D53" s="1" t="n"/>
+      <c r="E53" s="1" t="n"/>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="77">
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:F4"/>
@@ -771,6 +971,45 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -792,31 +1031,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -824,7 +1063,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -853,7 +1092,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -882,7 +1121,7 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -911,7 +1150,7 @@
         <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -956,31 +1195,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -988,7 +1227,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -1017,7 +1256,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -1046,7 +1285,7 @@
         <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -1091,31 +1330,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1123,7 +1362,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -1168,16 +1407,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1201,92 +1440,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casi terminada la interfaz gráfica
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -544,36 +544,57 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="2" t="n"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="n">
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n">
         <v>195</v>
       </c>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="n">
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n">
         <v>515.4</v>
       </c>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="n">
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
         <v>710.4</v>
       </c>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="n">
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n">
         <v>21.81</v>
       </c>
     </row>
@@ -581,52 +602,81 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="n">
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
         <v>37.5</v>
       </c>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="n">
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
         <v>135.5</v>
       </c>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="n">
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n">
         <v>173</v>
       </c>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="2" t="n"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="n">
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n">
         <v>5.31</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="n">
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n">
         <v>157.5</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="n">
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n">
         <v>4.84</v>
       </c>
     </row>
@@ -634,80 +684,126 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" t="n">
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
         <v>945</v>
       </c>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="n">
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n">
         <v>1745.4</v>
       </c>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="n">
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
         <v>900</v>
       </c>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="2" t="n"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D19" t="n">
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n">
         <v>3590.4</v>
       </c>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" t="n">
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="2" t="n"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" t="n">
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n">
         <v>415.4</v>
       </c>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="n">
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="2" t="n"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
       <c r="D24" s="2" t="n">
         <v>515.4</v>
       </c>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n"/>
+      <c r="E25" s="2" t="n"/>
       <c r="F25" s="2" t="n">
         <v>488.5525634765625</v>
       </c>
@@ -716,14 +812,23 @@
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
       <c r="F26" s="2" t="n">
         <v>610.4</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="2" t="n"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
@@ -736,34 +841,50 @@
       <c r="F30" s="2" t="n"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D31" t="n">
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n">
         <v>195</v>
       </c>
+      <c r="E31" s="2" t="n"/>
+      <c r="F31" s="2" t="n"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="n">
+      <c r="B32" s="2" t="n"/>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="2" t="n">
         <v>385.68</v>
       </c>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="2" t="n"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D33" t="n">
+      <c r="B33" s="2" t="n"/>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n">
         <v>580.6800000000001</v>
       </c>
+      <c r="E33" s="2" t="n"/>
+      <c r="F33" s="2" t="n"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F34" t="n">
+      <c r="B34" s="2" t="n"/>
+      <c r="C34" s="2" t="n"/>
+      <c r="D34" s="2" t="n"/>
+      <c r="E34" s="2" t="n"/>
+      <c r="F34" s="2" t="n">
         <v>17.83</v>
       </c>
     </row>
@@ -778,50 +899,74 @@
       <c r="F35" s="2" t="n"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D36" t="n">
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n">
         <v>37.5</v>
       </c>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D37" t="n">
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n">
         <v>135.5</v>
       </c>
+      <c r="E37" s="2" t="n"/>
+      <c r="F37" s="2" t="n"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" t="n">
+      <c r="B38" s="2" t="n"/>
+      <c r="C38" s="2" t="n"/>
+      <c r="D38" s="2" t="n">
         <v>173</v>
       </c>
+      <c r="E38" s="2" t="n"/>
+      <c r="F38" s="2" t="n"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F39" t="n">
+      <c r="B39" s="2" t="n"/>
+      <c r="C39" s="2" t="n"/>
+      <c r="D39" s="2" t="n"/>
+      <c r="E39" s="2" t="n"/>
+      <c r="F39" s="2" t="n">
         <v>5.31</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F40" t="n">
+      <c r="B40" s="2" t="n"/>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n"/>
+      <c r="E40" s="2" t="n"/>
+      <c r="F40" s="2" t="n">
         <v>157.5</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F41" t="n">
+      <c r="B41" s="2" t="n"/>
+      <c r="C41" s="2" t="n"/>
+      <c r="D41" s="2" t="n"/>
+      <c r="E41" s="2" t="n"/>
+      <c r="F41" s="2" t="n">
         <v>4.84</v>
       </c>
     </row>
@@ -836,36 +981,52 @@
       <c r="F42" s="2" t="n"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D43" t="n">
+      <c r="B43" s="2" t="n"/>
+      <c r="C43" s="2" t="n"/>
+      <c r="D43" s="2" t="n">
         <v>945</v>
       </c>
+      <c r="E43" s="2" t="n"/>
+      <c r="F43" s="2" t="n"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D44" t="n">
+      <c r="B44" s="2" t="n"/>
+      <c r="C44" s="2" t="n"/>
+      <c r="D44" s="2" t="n">
         <v>1615.67</v>
       </c>
+      <c r="E44" s="2" t="n"/>
+      <c r="F44" s="2" t="n"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D45" t="n">
+      <c r="B45" s="2" t="n"/>
+      <c r="C45" s="2" t="n"/>
+      <c r="D45" s="2" t="n">
         <v>900</v>
       </c>
+      <c r="E45" s="2" t="n"/>
+      <c r="F45" s="2" t="n"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D46" t="n">
+      <c r="B46" s="2" t="n"/>
+      <c r="C46" s="2" t="n"/>
+      <c r="D46" s="2" t="n">
         <v>3460.67</v>
       </c>
+      <c r="E46" s="2" t="n"/>
+      <c r="F46" s="2" t="n"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
@@ -878,28 +1039,40 @@
       <c r="F47" s="2" t="n"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D48" t="n">
+      <c r="B48" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="E48" s="2" t="n"/>
+      <c r="F48" s="2" t="n"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D49" t="n">
+      <c r="B49" s="2" t="n"/>
+      <c r="C49" s="2" t="n"/>
+      <c r="D49" s="2" t="n">
         <v>285.67</v>
       </c>
+      <c r="E49" s="2" t="n"/>
+      <c r="F49" s="2" t="n"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D50" t="n">
+      <c r="B50" s="2" t="n"/>
+      <c r="C50" s="2" t="n"/>
+      <c r="D50" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="E50" s="2" t="n"/>
+      <c r="F50" s="2" t="n"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">

</xml_diff>